<commit_message>
Coding Grigala://   -  _  -
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -111,102 +111,42 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
-        <v>2131</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>10213</v>
+        <v>2222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>5032</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>9908</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>4024</v>
+        <v>5555</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
-        <v>40214</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>8194</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>96241</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>8324</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>2121</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>17213</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>6321</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>92908</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>14024</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>42214</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>82194</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>9641</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>28324</v>
+        <v>6666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>